<commit_message>
last commit of the day
</commit_message>
<xml_diff>
--- a/StücklisteMP.xlsx
+++ b/StücklisteMP.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Position</t>
   </si>
@@ -147,6 +147,15 @@
   </si>
   <si>
     <t>Load Switch IC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">863-MC74VHC1G135DBVT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAND Gatter </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC74VHC1G135DBVT1G </t>
   </si>
 </sst>
 </file>
@@ -782,7 +791,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,13 +1062,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="33" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="G12" s="6"/>
       <c r="H12" s="36"/>
       <c r="I12" s="37">

</xml_diff>